<commit_message>
Enhance cloud compatibility by adding folder selection logic and updating export methods for Excel and PDF files
</commit_message>
<xml_diff>
--- a/Data/Ausschreibungs-LV (Blanko) - Rölsdorfstraße - Abbrucharbeiten - 30102025.xlsx
+++ b/Data/Ausschreibungs-LV (Blanko) - Rölsdorfstraße - Abbrucharbeiten - 30102025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniduede-my.sharepoint.com/personal/mohamed_senhaby_stud_uni-due_de/Documents/PersonalWork/Laith/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{B6DEDA7F-B8CC-4FBF-81BE-7DE6F2C3D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE58E769-A552-4040-A355-EDB47F0C941C}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{B6DEDA7F-B8CC-4FBF-81BE-7DE6F2C3D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8D94E75-5273-4EDC-90BA-E3E818BECCE7}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,7 +659,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -798,16 +798,15 @@
         <v>21</v>
       </c>
       <c r="G7" s="3">
-        <f>SUMPRODUCT((Kalkulation!A2:A50000=B7)*Kalkulation!D2:D50000)</f>
-        <v>0</v>
+        <v>5450.65</v>
       </c>
       <c r="H7" s="3">
         <f>G7*E7</f>
-        <v>0</v>
+        <v>5450.65</v>
       </c>
       <c r="J7" s="3">
         <f>H7*(1-I7)</f>
-        <v>0</v>
+        <v>5450.65</v>
       </c>
       <c r="K7" s="4">
         <f>B2</f>
@@ -840,16 +839,15 @@
         <v>21</v>
       </c>
       <c r="G8" s="3">
-        <f>SUMPRODUCT((Kalkulation!A2:A50000=B8)*Kalkulation!D2:D50000)</f>
-        <v>0</v>
+        <v>246170.45</v>
       </c>
       <c r="H8" s="3">
         <f>G8*E8</f>
-        <v>0</v>
+        <v>246170.45</v>
       </c>
       <c r="J8" s="3">
         <f>H8*(1-I8)</f>
-        <v>0</v>
+        <v>246170.45</v>
       </c>
       <c r="K8" s="4">
         <f>B2</f>
@@ -878,12 +876,12 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15">
         <f>SUMIF(L:L,"3e936996-abc5-483d-a773-57262ced8b2c",J:J)</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="15">
         <f>H9*(1-I9)</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="6" t="s">
@@ -909,12 +907,12 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15">
         <f>SUMIF(L:L,"8dcdc5f3-6d59-460f-b33e-45ff2e36bedc",J:J)</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="15">
         <f>H10*(1-I10)</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="K10" s="16"/>
       <c r="L10" s="6" t="s">
@@ -936,12 +934,12 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15">
         <f>SUMIF(L:L,"b9639df7-2450-4743-a8d5-b925b24f98e8",J:J)</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="15">
         <f>(1-I11)*H11</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
       <c r="K11" s="16"/>
       <c r="L11" s="6"/>
@@ -965,7 +963,7 @@
       </c>
       <c r="J13" s="10">
         <f>(1+$B$2)*J11</f>
-        <v>0</v>
+        <v>251621.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>